<commit_message>
Update regression test plans Remove Feedback confirmation test Add Mobile App Support test
</commit_message>
<xml_diff>
--- a/scripts/codemagic-ci/testing/Regression-Test-Plan-Template-Android-PROD.xlsx
+++ b/scripts/codemagic-ci/testing/Regression-Test-Plan-Template-Android-PROD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbryant/Downloads/test_plans/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cbryant/UCSD/Dev/Flutter/campusmobile/scripts/codemagic-ci/testing/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B22F7E8C-BE10-A349-B8A1-E0079520BCDE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C36082B3-4413-2A4F-86EE-A9827EA968F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37960" yWindow="500" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-34740" yWindow="820" windowWidth="38400" windowHeight="19960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Regression Test Plan" sheetId="1" r:id="rId1"/>
@@ -77,9 +77,6 @@
   </si>
   <si>
     <t>PASS:</t>
-  </si>
-  <si>
-    <t>Feedback feature sends an email and the email is received</t>
   </si>
   <si>
     <t>FAIL:</t>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t>Barcode Generator (2D) - Invalid Barcode</t>
+  </si>
+  <si>
+    <t>Mobile App Support request creates SNOW ticket and email confirmation received</t>
   </si>
 </sst>
 </file>
@@ -1133,7 +1133,9 @@
   </sheetPr>
   <dimension ref="A1:V977"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
@@ -1382,13 +1384,13 @@
     </row>
     <row r="9" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
-        <v>19</v>
+        <v>74</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="3"/>
       <c r="D9" s="35"/>
       <c r="E9" s="32" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F9" s="28"/>
       <c r="G9" s="35"/>
@@ -1410,13 +1412,13 @@
     </row>
     <row r="10" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="3"/>
       <c r="D10" s="35"/>
       <c r="E10" s="32" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F10" s="29"/>
       <c r="G10" s="35"/>
@@ -1438,13 +1440,13 @@
     </row>
     <row r="11" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="3"/>
       <c r="D11" s="35"/>
       <c r="E11" s="32" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="30"/>
       <c r="G11" s="35"/>
@@ -1466,7 +1468,7 @@
     </row>
     <row r="12" spans="1:22" ht="30" x14ac:dyDescent="0.15">
       <c r="A12" s="52" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -1492,13 +1494,13 @@
     </row>
     <row r="13" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
       <c r="D13" s="35"/>
       <c r="E13" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="26"/>
       <c r="G13" s="35"/>
@@ -1520,13 +1522,13 @@
     </row>
     <row r="14" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A14" s="7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="35"/>
       <c r="E14" s="37" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="34"/>
       <c r="G14" s="35"/>
@@ -1548,13 +1550,13 @@
     </row>
     <row r="15" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A15" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
       <c r="D15" s="35"/>
       <c r="E15" s="53" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F15" s="34"/>
       <c r="G15" s="35"/>
@@ -1576,13 +1578,13 @@
     </row>
     <row r="16" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A16" s="7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
       <c r="D16" s="35"/>
       <c r="E16" s="54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F16" s="34"/>
       <c r="G16" s="35"/>
@@ -1604,13 +1606,13 @@
     </row>
     <row r="17" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
       <c r="D17" s="35"/>
       <c r="E17" s="53" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G17" s="35"/>
       <c r="H17" s="1"/>
@@ -1631,13 +1633,13 @@
     </row>
     <row r="18" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A18" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="35"/>
       <c r="E18" s="54" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F18" s="35"/>
       <c r="G18" s="35"/>
@@ -1659,13 +1661,13 @@
     </row>
     <row r="19" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A19" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B19" s="3"/>
       <c r="C19" s="3"/>
       <c r="D19" s="1"/>
       <c r="E19" s="53" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1687,13 +1689,13 @@
     </row>
     <row r="20" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="3"/>
       <c r="C20" s="3"/>
       <c r="D20" s="1"/>
       <c r="E20" s="54" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1715,7 +1717,7 @@
     </row>
     <row r="21" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A21" s="7" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B21" s="3"/>
       <c r="C21" s="3"/>
@@ -1741,7 +1743,7 @@
     </row>
     <row r="22" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A22" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22" s="3"/>
       <c r="C22" s="3"/>
@@ -1767,7 +1769,7 @@
     </row>
     <row r="23" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A23" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B23" s="3"/>
       <c r="C23" s="3"/>
@@ -1793,7 +1795,7 @@
     </row>
     <row r="24" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A24" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="3"/>
@@ -1818,7 +1820,7 @@
     </row>
     <row r="25" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A25" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -1843,7 +1845,7 @@
     </row>
     <row r="26" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A26" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -1869,7 +1871,7 @@
     </row>
     <row r="27" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A27" s="48" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="50"/>
       <c r="C27" s="50"/>
@@ -1895,7 +1897,7 @@
     </row>
     <row r="28" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A28" s="49" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B28" s="51"/>
       <c r="C28" s="51"/>
@@ -1921,7 +1923,7 @@
     </row>
     <row r="29" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A29" s="48" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B29" s="50"/>
       <c r="C29" s="50"/>
@@ -1946,7 +1948,7 @@
     </row>
     <row r="30" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A30" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1971,7 +1973,7 @@
     </row>
     <row r="31" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A31" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -1997,7 +1999,7 @@
     </row>
     <row r="32" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A32" s="7" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -2023,7 +2025,7 @@
     </row>
     <row r="33" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A33" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -2049,7 +2051,7 @@
     </row>
     <row r="34" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A34" s="7" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -2075,7 +2077,7 @@
     </row>
     <row r="35" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A35" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -2101,7 +2103,7 @@
     </row>
     <row r="36" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A36" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -2127,7 +2129,7 @@
     </row>
     <row r="37" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A37" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B37" s="3"/>
       <c r="C37" s="3"/>
@@ -2152,7 +2154,7 @@
     </row>
     <row r="38" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A38" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B38" s="3"/>
       <c r="C38" s="3"/>
@@ -2178,7 +2180,7 @@
     </row>
     <row r="39" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A39" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B39" s="3"/>
       <c r="C39" s="3"/>
@@ -2204,7 +2206,7 @@
     </row>
     <row r="40" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A40" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B40" s="10"/>
       <c r="C40" s="10"/>
@@ -2230,7 +2232,7 @@
     </row>
     <row r="41" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A41" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B41" s="3"/>
       <c r="C41" s="3"/>
@@ -2256,7 +2258,7 @@
     </row>
     <row r="42" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A42" s="7" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B42" s="3"/>
       <c r="C42" s="3"/>
@@ -2282,7 +2284,7 @@
     </row>
     <row r="43" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B43" s="10"/>
       <c r="C43" s="10"/>
@@ -2308,7 +2310,7 @@
     </row>
     <row r="44" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A44" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -2334,7 +2336,7 @@
     </row>
     <row r="45" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A45" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -2360,7 +2362,7 @@
     </row>
     <row r="46" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A46" s="7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -2386,7 +2388,7 @@
     </row>
     <row r="47" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A47" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B47" s="10"/>
       <c r="C47" s="10"/>
@@ -2412,7 +2414,7 @@
     </row>
     <row r="48" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A48" s="7" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B48" s="3"/>
       <c r="C48" s="3"/>
@@ -2438,7 +2440,7 @@
     </row>
     <row r="49" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A49" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B49" s="3"/>
       <c r="C49" s="3"/>
@@ -2464,7 +2466,7 @@
     </row>
     <row r="50" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A50" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -2490,7 +2492,7 @@
     </row>
     <row r="51" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A51" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -2516,7 +2518,7 @@
     </row>
     <row r="52" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A52" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B52" s="10"/>
       <c r="C52" s="10"/>
@@ -2542,7 +2544,7 @@
     </row>
     <row r="53" spans="1:22" ht="15" x14ac:dyDescent="0.15">
       <c r="A53" s="40" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B53" s="14"/>
       <c r="C53" s="3"/>
@@ -24761,18 +24763,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24959,18 +24961,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F950C44-5D9B-4216-BB47-9736F024226A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AF01965-4B53-4043-B5ED-A531E4D3A7B2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9AF01965-4B53-4043-B5ED-A531E4D3A7B2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8F950C44-5D9B-4216-BB47-9736F024226A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>